<commit_message>
alfa_id and alfa_iw added, now working here
</commit_message>
<xml_diff>
--- a/db_elements.xlsx
+++ b/db_elements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A2867C-B43A-4402-9393-745600C0E288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C70D5DCD-8616-47AF-9B00-B9DE15207907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EA0A321-E68E-4267-92E4-8AB0665A3B7C}"/>
+    <workbookView xWindow="4128" yWindow="1104" windowWidth="17280" windowHeight="8964" xr2:uid="{1EA0A321-E68E-4267-92E4-8AB0665A3B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Benceno</t>
   </si>
@@ -443,6 +443,46 @@
   </si>
   <si>
     <t>Pc</t>
+  </si>
+  <si>
+    <t>n-Octano</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>18</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -486,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -509,11 +549,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -521,6 +572,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -836,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109E2E51-D6E3-4243-A945-B9D688533928}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,6 +1136,29 @@
         <v>38.299999999999997</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4.0507499999999999</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1356.36</v>
+      </c>
+      <c r="E11" s="4">
+        <v>209.63499999999999</v>
+      </c>
+      <c r="F11" s="5">
+        <v>295.39999999999998</v>
+      </c>
+      <c r="G11">
+        <v>24.824629999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Burbuja is working, big changes added, fuck dict, viva deepcopy
</commit_message>
<xml_diff>
--- a/db_elements.xlsx
+++ b/db_elements.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sugey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C70D5DCD-8616-47AF-9B00-B9DE15207907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87F39A95-C8F2-B448-9B82-9BBE5B80BBB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4128" yWindow="1104" windowWidth="17280" windowHeight="8964" xr2:uid="{1EA0A321-E68E-4267-92E4-8AB0665A3B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="32">
   <si>
     <t>Benceno</t>
   </si>
@@ -286,6 +288,9 @@
     <t>o-Xileno</t>
   </si>
   <si>
+    <t>Cumeno</t>
+  </si>
+  <si>
     <r>
       <t>C</t>
     </r>
@@ -298,6 +303,67 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+  </si>
+  <si>
+    <t>Acetato de Etilo</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>8</t>
     </r>
     <r>
@@ -308,107 +374,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
-    </r>
-  </si>
-  <si>
-    <t>Cumeno</t>
-  </si>
-  <si>
-    <r>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12</t>
-    </r>
-  </si>
-  <si>
-    <t>Acetato de Etilo</t>
-  </si>
-  <si>
-    <r>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>O</t>
     </r>
     <r>
@@ -445,51 +410,26 @@
     <t>Pc</t>
   </si>
   <si>
+    <t>Pto.ebu</t>
+  </si>
+  <si>
+    <t>80,1</t>
+  </si>
+  <si>
+    <t>C8H18</t>
+  </si>
+  <si>
     <t>n-Octano</t>
   </si>
   <si>
-    <r>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>18</t>
-    </r>
+    <t>C8H10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,8 +451,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +469,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -573,12 +526,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,271 +855,307 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109E2E51-D6E3-4243-A945-B9D688533928}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.23828125" customWidth="1"/>
+    <col min="2" max="2" width="11.02734375" customWidth="1"/>
+    <col min="7" max="7" width="9.55078125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.87109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.9540500000000001</v>
+      </c>
+      <c r="D2" s="1">
+        <v>663.72</v>
+      </c>
+      <c r="E2" s="1">
+        <v>256.68099999999998</v>
+      </c>
+      <c r="F2" s="1">
+        <v>32.4056</v>
+      </c>
+      <c r="G2" s="1">
+        <v>48.938986999999997</v>
+      </c>
+      <c r="H2" s="6">
+        <v>-89</v>
+      </c>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.9326599999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>935.77300000000002</v>
+      </c>
+      <c r="E3" s="1">
+        <v>238.78899999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>152</v>
+      </c>
+      <c r="G3" s="1">
+        <v>37.969428000000001</v>
+      </c>
+      <c r="H3" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.2183999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1197.01</v>
+      </c>
+      <c r="E4" s="1">
+        <v>228.06</v>
+      </c>
+      <c r="F4" s="1">
+        <v>235.05</v>
+      </c>
+      <c r="G4" s="1">
+        <v>47.0061407428</v>
+      </c>
+      <c r="H4" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.0013899999999998</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1170.875</v>
+      </c>
+      <c r="E5" s="1">
+        <v>224.31700000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>235</v>
+      </c>
+      <c r="G5" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="H5" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.13361</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1195.1300000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>212.47</v>
+      </c>
+      <c r="F6" s="1">
+        <v>250.1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="H6" s="6">
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C7" s="1">
         <v>3.9852300000000001</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D7" s="1">
         <v>1184.24</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E7" s="1">
         <v>217.572</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F7" s="1">
         <v>289.01</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G7" s="1">
         <v>48.990637</v>
       </c>
+      <c r="H7" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4.2183999999999999</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1197.01</v>
-      </c>
-      <c r="E3" s="1">
-        <v>228.06</v>
-      </c>
-      <c r="F3" s="1">
-        <v>235.05</v>
-      </c>
-      <c r="G3" s="1">
-        <v>47.0061407428</v>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.0202299999999997</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1263.9090000000001</v>
+      </c>
+      <c r="E8" s="1">
+        <v>216.43199999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>266.98</v>
+      </c>
+      <c r="G8" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="H8" s="6">
+        <v>98.42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.9326599999999998</v>
-      </c>
-      <c r="D4" s="1">
-        <v>935.77300000000002</v>
-      </c>
-      <c r="E4" s="1">
-        <v>238.78899999999999</v>
-      </c>
-      <c r="F4" s="1">
-        <v>152</v>
-      </c>
-      <c r="G4" s="1">
-        <v>37.969428000000001</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>4.0507499999999999</v>
+      </c>
+      <c r="D9">
+        <v>1356.36</v>
+      </c>
+      <c r="E9">
+        <v>209.63499999999999</v>
+      </c>
+      <c r="F9">
+        <v>295.39999999999998</v>
+      </c>
+      <c r="G9">
+        <v>24.824629999999999</v>
+      </c>
+      <c r="H9" s="8">
+        <v>125.6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3.9540500000000001</v>
-      </c>
-      <c r="D5" s="1">
-        <v>663.72</v>
-      </c>
-      <c r="E5" s="1">
-        <v>256.68099999999998</v>
-      </c>
-      <c r="F5" s="1">
-        <v>32.4056</v>
-      </c>
-      <c r="G5" s="1">
-        <v>48.938986999999997</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.0978899999999996</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1458.7059999999999</v>
+      </c>
+      <c r="E10" s="1">
+        <v>212.041</v>
+      </c>
+      <c r="F10" s="1">
+        <v>357.2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>37</v>
+      </c>
+      <c r="H10" s="6">
+        <v>138.4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="C11" s="1">
         <v>4.0611199999999998</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D11" s="1">
         <v>1460.7660000000001</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E11" s="1">
         <v>207.83</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F11" s="1">
         <v>357.9</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G11" s="1">
         <v>32.089627</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4.0202299999999997</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1263.9090000000001</v>
-      </c>
-      <c r="E7" s="1">
-        <v>216.43199999999999</v>
-      </c>
-      <c r="F7" s="1">
-        <v>266.98</v>
-      </c>
-      <c r="G7" s="1">
-        <v>27.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.0013899999999998</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1170.875</v>
-      </c>
-      <c r="E8" s="1">
-        <v>224.31700000000001</v>
-      </c>
-      <c r="F8" s="1">
-        <v>235</v>
-      </c>
-      <c r="G8" s="1">
-        <v>29.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4.0978899999999996</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1458.7059999999999</v>
-      </c>
-      <c r="E9" s="1">
-        <v>212.041</v>
-      </c>
-      <c r="F9" s="1">
-        <v>357.2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4.13361</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1195.1300000000001</v>
-      </c>
-      <c r="E10" s="1">
-        <v>212.47</v>
-      </c>
-      <c r="F10" s="1">
-        <v>250.1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>38.299999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4">
-        <v>4.0507499999999999</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1356.36</v>
-      </c>
-      <c r="E11" s="4">
-        <v>209.63499999999999</v>
-      </c>
-      <c r="F11" s="5">
-        <v>295.39999999999998</v>
-      </c>
-      <c r="G11">
-        <v>24.824629999999999</v>
+      <c r="H11" s="6">
+        <v>152.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>